<commit_message>
Update OOXML, creates basic order table
OOXML from 1.0 to 1.1, XSSFTester creates 3x9 table for orders to go in,
but file seems to be mysteriously "corrupted" every time after running
program
</commit_message>
<xml_diff>
--- a/XSSFTEST.xlsx
+++ b/XSSFTEST.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="4">
   <si>
-    <t>Column0</t>
+    <t>First Name</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Last Name</t>
   </si>
   <si>
-    <t>Column2</t>
+    <t>Special #</t>
   </si>
   <si>
     <t>0</t>
@@ -67,11 +67,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Test" ref="A1:C3" id="1" name="Test" totalsRowCount="1">
-  <tableColumns count="3">
-    <tableColumn name="Column0" id="1"/>
-    <tableColumn name="Column1" id="2"/>
-    <tableColumn name="Column2" id="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Test" ref="A1:J3" id="1" name="Test" totalsRowCount="1">
+  <tableColumns count="9">
+    <tableColumn name="First Name" id="1"/>
+    <tableColumn name="Last Name" id="2"/>
+    <tableColumn name="Special #" id="3"/>
+    <tableColumn name="Column" id="4"/>
+    <tableColumn name="Column" id="5"/>
+    <tableColumn name="Column" id="6"/>
+    <tableColumn name="Column" id="7"/>
+    <tableColumn name="Column" id="8"/>
+    <tableColumn name="Column" id="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showColumnStripes="false" showRowStripes="true"/>
 </table>
@@ -118,6 +124,72 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts>

</xml_diff>